<commit_message>
new datset tried on lstm AMOCARE CV 625
</commit_message>
<xml_diff>
--- a/outputs/forecast_MEFORNIX-P_TAB_8weeks_LSTM.xlsx
+++ b/outputs/forecast_MEFORNIX-P_TAB_8weeks_LSTM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,46 +485,6 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-W47</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-W48</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-W49</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-W50</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>358</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>